<commit_message>
adding Augur SQL queries
</commit_message>
<xml_diff>
--- a/data/repo_list/2nd_collection_repo_URLs_FINAL copy.xlsx
+++ b/data/repo_list/2nd_collection_repo_URLs_FINAL copy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul/Documents/08 - Hertie/thesis_stf/data/repo_list/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulsharratt/Documents/Hertie/Semester 4/03 - Master's Thesis/thesis_stf/data/repo_list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2611A3F3-5C5D-B447-9185-570B0742C0D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C457636-4FA3-594E-B93F-8376861257C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="5900" windowWidth="27640" windowHeight="16940" xr2:uid="{9CBEB7CE-B211-344B-BFDA-A8E95577DA04}"/>
+    <workbookView xWindow="-2040" yWindow="-20740" windowWidth="27640" windowHeight="16440" xr2:uid="{9CBEB7CE-B211-344B-BFDA-A8E95577DA04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>https://github.com/GNOME/libxml2/</t>
   </si>
@@ -70,9 +70,6 @@
     <t xml:space="preserve">https://github.com/openjs-foundation/ </t>
   </si>
   <si>
-    <t xml:space="preserve"> https://github.com/rubygems/rubygems/tree/master/bundler</t>
-  </si>
-  <si>
     <t>https://github.com/pypi/warehouse/</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
     <t>https://github.com/uutils/coreutils/</t>
   </si>
   <si>
-    <t>https://github.com/sequoia-pgp/</t>
-  </si>
-  <si>
     <t>https://github.com/fortran-lang/fpm/</t>
   </si>
   <si>
@@ -140,13 +134,22 @@
   </si>
   <si>
     <t>https://github.com/sigstore/protobuf-specs/</t>
+  </si>
+  <si>
+    <t>Included</t>
+  </si>
+  <si>
+    <t>Removed</t>
+  </si>
+  <si>
+    <t>https://github.com/sequoia-pgp/sequoia-git</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -158,6 +161,14 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -184,9 +195,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -206,9 +218,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -246,7 +258,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -352,7 +364,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -494,7 +506,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -502,122 +514,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{411F10CA-4BE3-C94B-A9D8-111363EDDCAF}">
-  <dimension ref="C4:C39"/>
+  <dimension ref="C3:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C39"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="J4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="J6" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="J7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="3:3" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C9" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="3:3" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C12" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="3:3" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C13" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="3:3" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C14" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="3:3" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C15" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="3:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C16" s="1" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C17" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C18" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C19" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C20" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C21" s="1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C22" s="1" t="s">
-        <v>24</v>
+      <c r="C22" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C24" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C25" t="s">
-        <v>6</v>
+      <c r="C25" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.2">
@@ -626,13 +658,13 @@
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C27" t="s">
-        <v>11</v>
+      <c r="C27" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C28" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="3:3" x14ac:dyDescent="0.2">
@@ -642,52 +674,27 @@
     </row>
     <row r="30" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C30" s="1" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C31" s="1" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C32" s="1" t="s">
-        <v>12</v>
+      <c r="C32" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C33" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C34" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C35" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C36" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C37" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C38" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C39" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -695,36 +702,36 @@
     <hyperlink ref="C4" r:id="rId1" xr:uid="{FE5EEC6D-25E3-CE46-A846-EB4A008BC115}"/>
     <hyperlink ref="C7" r:id="rId2" xr:uid="{511F5C58-0E23-444D-BF47-B1DE76C16878}"/>
     <hyperlink ref="C10" r:id="rId3" xr:uid="{C95A847D-DB9B-5945-9D46-E0BC022C7885}"/>
-    <hyperlink ref="C11" r:id="rId4" xr:uid="{EF5093F6-9432-2C43-8864-756B1C9F5DA6}"/>
-    <hyperlink ref="C14" r:id="rId5" xr:uid="{25CE9709-AAB6-EA43-ACA8-A104B51B4FF2}"/>
-    <hyperlink ref="C15" r:id="rId6" xr:uid="{BC767357-D057-E04E-B5AB-0898C7A469AE}"/>
-    <hyperlink ref="C17" r:id="rId7" xr:uid="{1959B640-5BC0-2F46-A473-631F68CAA9AD}"/>
-    <hyperlink ref="C18" r:id="rId8" xr:uid="{0B19CFF2-9401-C146-A241-10645006F954}"/>
-    <hyperlink ref="C23" r:id="rId9" xr:uid="{4369FBE7-F098-C94C-A76B-B3867D26E1A9}"/>
-    <hyperlink ref="C24" r:id="rId10" xr:uid="{AEEF9057-A9EA-584B-B617-B6FAB38AFF7A}"/>
-    <hyperlink ref="C26" r:id="rId11" xr:uid="{56AFF563-B099-E941-A522-281B86890875}"/>
-    <hyperlink ref="C28" r:id="rId12" xr:uid="{78A9CAA1-3302-CB45-8008-D8A906FD36FA}"/>
-    <hyperlink ref="C31" r:id="rId13" xr:uid="{804DDFCA-3B0E-EE45-BB30-7D6220A516D6}"/>
-    <hyperlink ref="C34" r:id="rId14" xr:uid="{30C1F1FE-66F3-DC49-B59B-1474B17ACAAF}"/>
+    <hyperlink ref="J4" r:id="rId4" xr:uid="{EF5093F6-9432-2C43-8864-756B1C9F5DA6}"/>
+    <hyperlink ref="C12" r:id="rId5" xr:uid="{25CE9709-AAB6-EA43-ACA8-A104B51B4FF2}"/>
+    <hyperlink ref="C13" r:id="rId6" xr:uid="{BC767357-D057-E04E-B5AB-0898C7A469AE}"/>
+    <hyperlink ref="J7" r:id="rId7" xr:uid="{1959B640-5BC0-2F46-A473-631F68CAA9AD}"/>
+    <hyperlink ref="C15" r:id="rId8" xr:uid="{0B19CFF2-9401-C146-A241-10645006F954}"/>
+    <hyperlink ref="C20" r:id="rId9" xr:uid="{4369FBE7-F098-C94C-A76B-B3867D26E1A9}"/>
+    <hyperlink ref="C21" r:id="rId10" xr:uid="{AEEF9057-A9EA-584B-B617-B6FAB38AFF7A}"/>
+    <hyperlink ref="C23" r:id="rId11" xr:uid="{56AFF563-B099-E941-A522-281B86890875}"/>
+    <hyperlink ref="C24" r:id="rId12" xr:uid="{78A9CAA1-3302-CB45-8008-D8A906FD36FA}"/>
+    <hyperlink ref="C27" r:id="rId13" xr:uid="{804DDFCA-3B0E-EE45-BB30-7D6220A516D6}"/>
+    <hyperlink ref="C30" r:id="rId14" xr:uid="{30C1F1FE-66F3-DC49-B59B-1474B17ACAAF}"/>
     <hyperlink ref="C5" r:id="rId15" xr:uid="{491D24B4-9AB5-8F42-A7EC-7EA7D8982240}"/>
     <hyperlink ref="C8" r:id="rId16" xr:uid="{3B0C2E59-A77D-1546-A4CC-2622E2BC12D7}"/>
-    <hyperlink ref="C12" r:id="rId17" xr:uid="{35CEC77A-D100-8E4D-960A-CDFCA8FE39BB}"/>
-    <hyperlink ref="C16" r:id="rId18" xr:uid="{39A33E2F-B543-3D41-A3B4-F73B01CBEC1C}"/>
-    <hyperlink ref="C29" r:id="rId19" xr:uid="{1F4B9FEA-25FA-EF4F-B122-BACD2479AC0B}"/>
-    <hyperlink ref="C30" r:id="rId20" xr:uid="{3C3900B9-4440-0946-BF51-84D889CAA1F5}"/>
-    <hyperlink ref="C35" r:id="rId21" xr:uid="{283AAA90-5FBF-1340-B721-5129CAE8ECE5}"/>
+    <hyperlink ref="J5" r:id="rId17" xr:uid="{35CEC77A-D100-8E4D-960A-CDFCA8FE39BB}"/>
+    <hyperlink ref="C14" r:id="rId18" xr:uid="{39A33E2F-B543-3D41-A3B4-F73B01CBEC1C}"/>
+    <hyperlink ref="C25" r:id="rId19" xr:uid="{1F4B9FEA-25FA-EF4F-B122-BACD2479AC0B}"/>
+    <hyperlink ref="C26" r:id="rId20" xr:uid="{3C3900B9-4440-0946-BF51-84D889CAA1F5}"/>
+    <hyperlink ref="J6" r:id="rId21" xr:uid="{283AAA90-5FBF-1340-B721-5129CAE8ECE5}"/>
     <hyperlink ref="C9" r:id="rId22" xr:uid="{58A0F2C1-6414-4645-9D2B-C9C83D2FFFA6}"/>
-    <hyperlink ref="C21" r:id="rId23" xr:uid="{4C5343D4-5157-9241-B2DF-858D3B22A4ED}"/>
-    <hyperlink ref="C22" r:id="rId24" xr:uid="{0CBE5ECC-83A7-D84A-A499-FA72E7D314D8}"/>
-    <hyperlink ref="C38" r:id="rId25" xr:uid="{B577758A-E9F7-DB41-BC1B-74E57E7D1E2B}"/>
+    <hyperlink ref="C18" r:id="rId23" xr:uid="{4C5343D4-5157-9241-B2DF-858D3B22A4ED}"/>
+    <hyperlink ref="C19" r:id="rId24" xr:uid="{0CBE5ECC-83A7-D84A-A499-FA72E7D314D8}"/>
+    <hyperlink ref="C33" r:id="rId25" xr:uid="{B577758A-E9F7-DB41-BC1B-74E57E7D1E2B}"/>
     <hyperlink ref="C6" r:id="rId26" xr:uid="{2736A8FE-BF34-8248-A2EF-15AA385ABE37}"/>
-    <hyperlink ref="C13" r:id="rId27" xr:uid="{0B0BF968-2DDA-C449-B5DD-83C5029695C1}"/>
-    <hyperlink ref="C19" r:id="rId28" xr:uid="{CF992959-F153-0E45-BF0F-EFB864AE8765}"/>
-    <hyperlink ref="C20" r:id="rId29" xr:uid="{22317C03-9F3B-2046-B673-946094BC7B50}"/>
-    <hyperlink ref="C32" r:id="rId30" xr:uid="{EB39D112-D958-254C-A946-412C1FAC4504}"/>
-    <hyperlink ref="C33" r:id="rId31" xr:uid="{6C857812-6FFD-3645-9771-599DCB7A2EAD}"/>
-    <hyperlink ref="C36" r:id="rId32" xr:uid="{F30DCCA3-2FFA-B840-ABF0-BDB098CA3BF2}"/>
-    <hyperlink ref="C39" r:id="rId33" xr:uid="{7136531E-5E08-0A40-9163-12C1ABD9FC04}"/>
+    <hyperlink ref="C11" r:id="rId27" xr:uid="{0B0BF968-2DDA-C449-B5DD-83C5029695C1}"/>
+    <hyperlink ref="C16" r:id="rId28" xr:uid="{CF992959-F153-0E45-BF0F-EFB864AE8765}"/>
+    <hyperlink ref="C17" r:id="rId29" xr:uid="{22317C03-9F3B-2046-B673-946094BC7B50}"/>
+    <hyperlink ref="C28" r:id="rId30" xr:uid="{EB39D112-D958-254C-A946-412C1FAC4504}"/>
+    <hyperlink ref="C29" r:id="rId31" xr:uid="{6C857812-6FFD-3645-9771-599DCB7A2EAD}"/>
+    <hyperlink ref="C31" r:id="rId32" xr:uid="{F30DCCA3-2FFA-B840-ABF0-BDB098CA3BF2}"/>
+    <hyperlink ref="C34" r:id="rId33" xr:uid="{7136531E-5E08-0A40-9163-12C1ABD9FC04}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>